<commit_message>
Ajout du jour 06.12.2018
</commit_message>
<xml_diff>
--- a/DOC/QRR_JDB.xlsx
+++ b/DOC/QRR_JDB.xlsx
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="Quentin" sheetId="1" r:id="rId1"/>
-    <sheet name="Philippe" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Quentin!$A$1:$E$38</definedName>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="147">
   <si>
     <t>Date</t>
   </si>
@@ -434,6 +433,36 @@
   </si>
   <si>
     <t>Documentation, écriture des parties restantes à faire et des tests</t>
+  </si>
+  <si>
+    <t>Discution et remise à jour du règlement de la formation avec M.Chevillat</t>
+  </si>
+  <si>
+    <t>Module et note éliminatoire</t>
+  </si>
+  <si>
+    <t>Diagrame d'activité</t>
+  </si>
+  <si>
+    <t>2 période ou presque de diagrame d'activité</t>
+  </si>
+  <si>
+    <t>11h50</t>
+  </si>
+  <si>
+    <t>Ajout, mise à jour de cartes</t>
+  </si>
+  <si>
+    <t>Carte à faire dans le futur proche</t>
+  </si>
+  <si>
+    <t>Prise de connaissance des période de présentation</t>
+  </si>
+  <si>
+    <t>Rédaction du plan de test complet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecriture du journal de bord et commit </t>
   </si>
 </sst>
 </file>
@@ -479,7 +508,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -639,20 +668,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -773,7 +793,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -781,71 +822,47 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1160,10 +1177,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,11 +1194,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="59"/>
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1190,9 +1207,9 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="64"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1234,12 +1251,12 @@
         <f>SUM(B8:B13)</f>
         <v>0.10069444444444445</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="56"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="65"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="65">
+      <c r="A8" s="66">
         <v>43343</v>
       </c>
       <c r="B8" s="31">
@@ -1252,7 +1269,7 @@
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="66"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1266,7 +1283,7 @@
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
+      <c r="A10" s="67"/>
       <c r="B10" s="23">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1277,7 +1294,7 @@
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="23">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1288,7 +1305,7 @@
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
+      <c r="A12" s="67"/>
       <c r="B12" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1299,7 +1316,7 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="66"/>
+      <c r="A13" s="67"/>
       <c r="B13" s="20">
         <v>3.125E-2</v>
       </c>
@@ -1317,14 +1334,14 @@
         <f>SUM(B15:B23)</f>
         <v>0.1875</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="65"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="57">
+      <c r="A15" s="50">
         <v>43347</v>
       </c>
       <c r="B15" s="29">
@@ -1339,7 +1356,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="23">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1351,7 +1368,7 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
+      <c r="A17" s="55"/>
       <c r="B17" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1363,7 +1380,7 @@
       <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1376,7 +1393,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="47">
+      <c r="A19" s="49">
         <v>43350</v>
       </c>
       <c r="B19" s="29">
@@ -1389,7 +1406,7 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1402,7 +1419,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="29">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1413,7 +1430,7 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="29">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1424,7 +1441,7 @@
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="49"/>
+      <c r="A23" s="56"/>
       <c r="B23" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1442,14 +1459,14 @@
         <f>SUM(B25:B29)</f>
         <v>9.375E-2</v>
       </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="56"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="65"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="57">
+      <c r="A25" s="50">
         <v>43354</v>
       </c>
       <c r="B25" s="24">
@@ -1464,7 +1481,7 @@
       <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
+      <c r="A26" s="55"/>
       <c r="B26" s="24">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1477,7 +1494,7 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
+      <c r="A27" s="55"/>
       <c r="B27" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1485,14 +1502,14 @@
         <v>34</v>
       </c>
       <c r="D27" s="16"/>
-      <c r="E27" s="67" t="s">
+      <c r="E27" s="68" t="s">
         <v>36</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
+      <c r="A28" s="55"/>
       <c r="B28" s="24">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1500,10 +1517,10 @@
         <v>35</v>
       </c>
       <c r="D28" s="16"/>
-      <c r="E28" s="67"/>
+      <c r="E28" s="68"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
+      <c r="A29" s="55"/>
       <c r="B29" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1511,11 +1528,11 @@
         <v>37</v>
       </c>
       <c r="D29" s="16"/>
-      <c r="E29" s="67"/>
+      <c r="E29" s="68"/>
       <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="47">
+      <c r="A30" s="49">
         <v>43357</v>
       </c>
       <c r="B30" s="24">
@@ -1529,7 +1546,7 @@
       <c r="G30" s="9"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
+      <c r="A31" s="49"/>
       <c r="B31" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1537,12 +1554,12 @@
         <v>39</v>
       </c>
       <c r="D31" s="16"/>
-      <c r="E31" s="67" t="s">
+      <c r="E31" s="68" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
+      <c r="A32" s="49"/>
       <c r="B32" s="24">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1550,10 +1567,10 @@
         <v>43</v>
       </c>
       <c r="D32" s="15"/>
-      <c r="E32" s="67"/>
+      <c r="E32" s="68"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
+      <c r="A33" s="49"/>
       <c r="B33" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1561,10 +1578,10 @@
         <v>42</v>
       </c>
       <c r="D33" s="15"/>
-      <c r="E33" s="67"/>
+      <c r="E33" s="68"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="49"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="25">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1579,11 +1596,11 @@
         <v>119</v>
       </c>
       <c r="B35" s="26"/>
-      <c r="C35" s="54" t="s">
+      <c r="C35" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="55"/>
-      <c r="E35" s="56"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="65"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="28" t="s">
@@ -1593,12 +1610,12 @@
         <f>SUM(B37:B47)</f>
         <v>0.1875</v>
       </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="56"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="65"/>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="57">
+      <c r="A37" s="50">
         <v>43368</v>
       </c>
       <c r="B37" s="24">
@@ -1615,7 +1632,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="48"/>
+      <c r="A38" s="55"/>
       <c r="B38" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1626,7 +1643,7 @@
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="48"/>
+      <c r="A39" s="55"/>
       <c r="B39" s="24">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1639,7 +1656,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
+      <c r="A40" s="55"/>
       <c r="B40" s="24">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1650,7 +1667,7 @@
       <c r="E40" s="13"/>
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="48"/>
+      <c r="A41" s="55"/>
       <c r="B41" s="24">
         <v>3.472222222222222E-3</v>
       </c>
@@ -1661,7 +1678,7 @@
       <c r="E41" s="13"/>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="48">
+      <c r="A42" s="55">
         <v>43371</v>
       </c>
       <c r="B42" s="24">
@@ -1674,7 +1691,7 @@
       <c r="E42" s="13"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="48"/>
+      <c r="A43" s="55"/>
       <c r="B43" s="24">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1687,7 +1704,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="48"/>
+      <c r="A44" s="55"/>
       <c r="B44" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1698,7 +1715,7 @@
       <c r="E44" s="13"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="48"/>
+      <c r="A45" s="55"/>
       <c r="B45" s="24">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1709,7 +1726,7 @@
       <c r="E45" s="13"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="48"/>
+      <c r="A46" s="55"/>
       <c r="B46" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1720,7 +1737,7 @@
       <c r="E46" s="13"/>
     </row>
     <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="49"/>
+      <c r="A47" s="56"/>
       <c r="B47" s="37">
         <v>3.472222222222222E-3</v>
       </c>
@@ -1738,12 +1755,12 @@
         <f>SUM(B49:B55)</f>
         <v>9.3750000000000014E-2</v>
       </c>
-      <c r="C48" s="54"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="56"/>
+      <c r="C48" s="63"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="65"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="57">
+      <c r="A49" s="50">
         <v>43375</v>
       </c>
       <c r="B49" s="24">
@@ -1758,7 +1775,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="48"/>
+      <c r="A50" s="55"/>
       <c r="B50" s="24">
         <v>2.4305555555555556E-2</v>
       </c>
@@ -1771,7 +1788,7 @@
       <c r="E50" s="13"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="48"/>
+      <c r="A51" s="55"/>
       <c r="B51" s="24">
         <v>3.472222222222222E-3</v>
       </c>
@@ -1782,7 +1799,7 @@
       <c r="E51" s="13"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="48"/>
+      <c r="A52" s="55"/>
       <c r="B52" s="24">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1793,7 +1810,7 @@
       <c r="E52" s="13"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="48"/>
+      <c r="A53" s="55"/>
       <c r="B53" s="24">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1801,12 +1818,12 @@
         <v>61</v>
       </c>
       <c r="D53" s="16"/>
-      <c r="E53" s="53" t="s">
+      <c r="E53" s="69" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="48"/>
+      <c r="A54" s="55"/>
       <c r="B54" s="24">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1814,7 +1831,7 @@
         <v>59</v>
       </c>
       <c r="D54" s="16"/>
-      <c r="E54" s="53"/>
+      <c r="E54" s="69"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="45">
@@ -1835,12 +1852,12 @@
         <f>SUM(B57:B65)</f>
         <v>0.1875</v>
       </c>
-      <c r="C56" s="54"/>
-      <c r="D56" s="55"/>
-      <c r="E56" s="56"/>
+      <c r="C56" s="63"/>
+      <c r="D56" s="64"/>
+      <c r="E56" s="65"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="57">
+      <c r="A57" s="50">
         <v>43382</v>
       </c>
       <c r="B57" s="24">
@@ -1853,7 +1870,7 @@
       <c r="E57" s="13"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="48"/>
+      <c r="A58" s="55"/>
       <c r="B58" s="24">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1864,7 +1881,7 @@
       <c r="E58" s="13"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="48"/>
+      <c r="A59" s="55"/>
       <c r="B59" s="24">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -1875,7 +1892,7 @@
       <c r="E59" s="13"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="48"/>
+      <c r="A60" s="55"/>
       <c r="B60" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1888,7 +1905,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="48"/>
+      <c r="A61" s="55"/>
       <c r="B61" s="24">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1901,7 +1918,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="48">
+      <c r="A62" s="55">
         <v>43385</v>
       </c>
       <c r="B62" s="24">
@@ -1914,7 +1931,7 @@
       <c r="E62" s="13"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="48"/>
+      <c r="A63" s="55"/>
       <c r="B63" s="24">
         <v>3.125E-2</v>
       </c>
@@ -1927,7 +1944,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="48"/>
+      <c r="A64" s="55"/>
       <c r="B64" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1938,7 +1955,7 @@
       <c r="E64" s="13"/>
     </row>
     <row r="65" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="49"/>
+      <c r="A65" s="56"/>
       <c r="B65" s="37">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1951,19 +1968,19 @@
       <c r="E65" s="14"/>
     </row>
     <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="71" t="s">
+      <c r="A66" s="48" t="s">
         <v>88</v>
       </c>
       <c r="B66" s="42">
         <f>SUM(B67:B73)</f>
         <v>0.15624999999999997</v>
       </c>
-      <c r="C66" s="50"/>
-      <c r="D66" s="51"/>
-      <c r="E66" s="52"/>
+      <c r="C66" s="52"/>
+      <c r="D66" s="53"/>
+      <c r="E66" s="54"/>
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="47">
+      <c r="A67" s="49">
         <v>43404</v>
       </c>
       <c r="B67" s="29">
@@ -1980,7 +1997,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="47"/>
+      <c r="A68" s="49"/>
       <c r="B68" s="29">
         <v>3.8194444444444441E-2</v>
       </c>
@@ -1995,7 +2012,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="48">
+      <c r="A69" s="55">
         <v>43406</v>
       </c>
       <c r="B69" s="29">
@@ -2007,7 +2024,7 @@
       <c r="E69" s="5"/>
     </row>
     <row r="70" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="48"/>
+      <c r="A70" s="55"/>
       <c r="B70" s="29">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -2020,7 +2037,7 @@
       <c r="E70" s="5"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="48"/>
+      <c r="A71" s="55"/>
       <c r="B71" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -2030,7 +2047,7 @@
       <c r="E71" s="5"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="48"/>
+      <c r="A72" s="55"/>
       <c r="B72" s="29">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -2040,7 +2057,7 @@
       <c r="E72" s="5"/>
     </row>
     <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="49"/>
+      <c r="A73" s="56"/>
       <c r="B73" s="43">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -2053,16 +2070,16 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="71" t="s">
+      <c r="A74" s="48" t="s">
         <v>106</v>
       </c>
       <c r="B74" s="42">
         <f>SUM(B76:B79)</f>
         <v>9.3749999999999986E-2</v>
       </c>
-      <c r="C74" s="50"/>
-      <c r="D74" s="51"/>
-      <c r="E74" s="52"/>
+      <c r="C74" s="52"/>
+      <c r="D74" s="53"/>
+      <c r="E74" s="54"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="46">
@@ -2074,7 +2091,7 @@
       <c r="E75" s="5"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="48">
+      <c r="A76" s="55">
         <v>43413</v>
       </c>
       <c r="B76" s="44">
@@ -2086,7 +2103,7 @@
       <c r="E76" s="5"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="48"/>
+      <c r="A77" s="55"/>
       <c r="B77" s="44">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -2096,7 +2113,7 @@
       <c r="E77" s="5"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="48"/>
+      <c r="A78" s="55"/>
       <c r="B78" s="44">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -2109,7 +2126,7 @@
       <c r="E78" s="5"/>
     </row>
     <row r="79" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="49"/>
+      <c r="A79" s="56"/>
       <c r="B79" s="43">
         <v>2.4305555555555556E-2</v>
       </c>
@@ -2122,16 +2139,16 @@
       <c r="E79" s="36"/>
     </row>
     <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="71" t="s">
+      <c r="A80" s="48" t="s">
         <v>107</v>
       </c>
       <c r="B80" s="42">
         <f>SUM(B82:B85)</f>
         <v>6.25E-2</v>
       </c>
-      <c r="C80" s="50"/>
-      <c r="D80" s="51"/>
-      <c r="E80" s="52"/>
+      <c r="C80" s="52"/>
+      <c r="D80" s="53"/>
+      <c r="E80" s="54"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="46">
@@ -2146,7 +2163,7 @@
       <c r="E81" s="5"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="47">
+      <c r="A82" s="49">
         <v>43420</v>
       </c>
       <c r="C82" t="s">
@@ -2158,7 +2175,7 @@
       <c r="E82" s="5"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="47"/>
+      <c r="A83" s="49"/>
       <c r="B83" s="29">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -2168,7 +2185,7 @@
       <c r="E83" s="5"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="47"/>
+      <c r="A84" s="49"/>
       <c r="B84" s="29">
         <v>2.4305555555555556E-2</v>
       </c>
@@ -2183,7 +2200,7 @@
       </c>
     </row>
     <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="47"/>
+      <c r="A85" s="49"/>
       <c r="B85" s="29">
         <v>3.125E-2</v>
       </c>
@@ -2193,19 +2210,19 @@
       <c r="E85" s="5"/>
     </row>
     <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="71" t="s">
+      <c r="A86" s="48" t="s">
         <v>116</v>
       </c>
       <c r="B86" s="42">
         <f>SUM(B87:B93)</f>
         <v>0.18749999999999997</v>
       </c>
-      <c r="C86" s="50"/>
-      <c r="D86" s="51"/>
-      <c r="E86" s="52"/>
+      <c r="C86" s="52"/>
+      <c r="D86" s="53"/>
+      <c r="E86" s="54"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="58">
+      <c r="A87" s="51">
         <v>43424</v>
       </c>
       <c r="B87" s="29">
@@ -2220,7 +2237,7 @@
       <c r="E87" s="5"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="58"/>
+      <c r="A88" s="51"/>
       <c r="B88" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -2230,7 +2247,7 @@
       <c r="E88" s="5"/>
     </row>
     <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="58"/>
+      <c r="A89" s="51"/>
       <c r="B89" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -2242,7 +2259,7 @@
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="58"/>
+      <c r="A90" s="51"/>
       <c r="B90" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -2252,7 +2269,7 @@
       <c r="E90" s="5"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="47">
+      <c r="A91" s="49">
         <v>43426</v>
       </c>
       <c r="B91" s="29">
@@ -2264,7 +2281,7 @@
       <c r="E91" s="5"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="47"/>
+      <c r="A92" s="49"/>
       <c r="B92" s="29">
         <v>4.8611111111111112E-2</v>
       </c>
@@ -2274,7 +2291,7 @@
       <c r="E92" s="5"/>
     </row>
     <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="47"/>
+      <c r="A93" s="49"/>
       <c r="B93" s="29">
         <v>2.4305555555555556E-2</v>
       </c>
@@ -2284,7 +2301,7 @@
       <c r="E93" s="5"/>
     </row>
     <row r="94" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="71" t="s">
+      <c r="A94" s="48" t="s">
         <v>127</v>
       </c>
       <c r="B94" s="42">
@@ -2314,17 +2331,17 @@
       <c r="E96" s="5"/>
     </row>
     <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="71" t="s">
+      <c r="A97" s="48" t="s">
         <v>128</v>
       </c>
       <c r="B97" s="42">
-        <f>SUM(B98:B101)</f>
+        <f>SUM(B98:B100)</f>
         <v>9.375E-2</v>
       </c>
       <c r="E97" s="5"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="57">
+      <c r="A98" s="50">
         <v>43438</v>
       </c>
       <c r="B98" s="29">
@@ -2336,7 +2353,7 @@
       <c r="E98" s="5"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="47"/>
+      <c r="A99" s="49"/>
       <c r="B99" s="29">
         <v>2.4305555555555556E-2</v>
       </c>
@@ -2346,7 +2363,7 @@
       <c r="E99" s="5"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="47"/>
+      <c r="A100" s="49"/>
       <c r="B100" s="29">
         <v>5.9027777777777783E-2</v>
       </c>
@@ -2356,31 +2373,69 @@
       <c r="E100" s="5"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="46">
+      <c r="A101" s="49">
         <v>43440</v>
       </c>
-      <c r="E101" s="5"/>
+      <c r="B101" s="29">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C101" t="s">
+        <v>137</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="46"/>
+      <c r="A102" s="49"/>
+      <c r="B102" s="29">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C102" t="s">
+        <v>139</v>
+      </c>
       <c r="E102" s="5"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E103" s="5"/>
+      <c r="A103" s="49"/>
+      <c r="B103" s="29">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="C103" t="s">
+        <v>142</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="30"/>
-      <c r="E104" s="5"/>
+      <c r="A104" s="49"/>
+      <c r="B104" s="29">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="C104" t="s">
+        <v>145</v>
+      </c>
+      <c r="E104" s="70" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="30"/>
+      <c r="A105" s="49"/>
+      <c r="B105" s="29">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C105" t="s">
+        <v>146</v>
+      </c>
+      <c r="E105" s="70"/>
     </row>
     <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="71" t="s">
+      <c r="A106" s="48" t="s">
         <v>129</v>
       </c>
       <c r="B106" s="42">
-        <f ca="1">SUM(B104:B107)</f>
+        <f ca="1">SUM(B104:B106)</f>
         <v>0</v>
       </c>
       <c r="C106" t="s">
@@ -2388,16 +2443,30 @@
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="30"/>
+      <c r="A107" s="47">
+        <v>43445</v>
+      </c>
+      <c r="B107" s="29"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="30"/>
+      <c r="A108" s="47">
+        <v>43447</v>
+      </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="30"/>
+      <c r="B109" s="29">
+        <v>0.15625</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="30"/>
+      <c r="B110" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C110" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="30"/>
@@ -2405,32 +2474,39 @@
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="30"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="30"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="30"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="30"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="30"/>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116" s="29">
+        <f>SUM(B101:B105)</f>
+        <v>0.15625</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="30"/>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="30"/>
+      <c r="B117" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A91:A93"/>
-    <mergeCell ref="A98:A100"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A23"/>
+  <mergeCells count="34">
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="A101:A105"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="C66:E66"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C14:E14"/>
@@ -2438,6 +2514,12 @@
     <mergeCell ref="E27:E29"/>
     <mergeCell ref="A25:A29"/>
     <mergeCell ref="C24:E24"/>
+    <mergeCell ref="A91:A93"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A23"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="E31:E33"/>
     <mergeCell ref="C56:E56"/>
@@ -2448,744 +2530,8 @@
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="A37:A41"/>
     <mergeCell ref="A42:A47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="C66:E66"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="68" fitToHeight="5" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H122"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="21"/>
-    <col min="2" max="2" width="9.5703125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="75.28515625" customWidth="1"/>
-    <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" customWidth="1"/>
-    <col min="6" max="6" width="58.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="21"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="21"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="32">
-        <f>SUM(B8:B13)</f>
-        <v>0.10069444444444445</v>
-      </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="56"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="65">
-        <v>43343</v>
-      </c>
-      <c r="B8" s="31">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="66"/>
-      <c r="B9" s="24">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
-      <c r="B10" s="23">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="13"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
-      <c r="B11" s="23">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
-      <c r="B12" s="23">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="13"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="66"/>
-      <c r="B13" s="20">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="26">
-        <f>SUM(B15:B23)</f>
-        <v>0.1875</v>
-      </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="57">
-        <v>43347</v>
-      </c>
-      <c r="B15" s="29">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
-      <c r="B16" s="23">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="13"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="23">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="13"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
-      <c r="B18" s="23">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="47">
-        <v>43350</v>
-      </c>
-      <c r="B19" s="29">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="29">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="29">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="29">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="49"/>
-      <c r="B23" s="23">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="14"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="56"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="57"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="13"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="13"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="13"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="13"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="68"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="19"/>
-      <c r="G29" s="9"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="69"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="70"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="B34"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-      <c r="B35"/>
-    </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-      <c r="B36"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-      <c r="B37"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-      <c r="B38"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="B39"/>
-    </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="B40"/>
-    </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-      <c r="B41"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42"/>
-      <c r="B42"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43"/>
-      <c r="B43"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44"/>
-      <c r="B44"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45"/>
-      <c r="B45"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46"/>
-      <c r="B46"/>
-    </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47"/>
-      <c r="B47"/>
-    </row>
-    <row r="48" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48"/>
-      <c r="B48"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49"/>
-      <c r="B49"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50"/>
-      <c r="B50"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51"/>
-      <c r="B51"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52"/>
-      <c r="B52"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53"/>
-      <c r="B53"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54"/>
-      <c r="B54"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55"/>
-      <c r="B55"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56"/>
-      <c r="B56"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57"/>
-      <c r="B57"/>
-    </row>
-    <row r="58" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58"/>
-      <c r="B58"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59"/>
-      <c r="B59"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60"/>
-      <c r="B60"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61"/>
-      <c r="B61"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62"/>
-      <c r="B62"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63"/>
-      <c r="B63"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64"/>
-      <c r="B64"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65"/>
-      <c r="B65"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66"/>
-      <c r="B66"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67"/>
-      <c r="B67"/>
-    </row>
-    <row r="68" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68"/>
-      <c r="B68"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69"/>
-      <c r="B69"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70"/>
-      <c r="B70"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71"/>
-      <c r="B71"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72"/>
-      <c r="B72"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73"/>
-      <c r="B73"/>
-    </row>
-    <row r="74" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74"/>
-      <c r="B74"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75"/>
-      <c r="B75"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76"/>
-      <c r="B76"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77"/>
-      <c r="B77"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78"/>
-      <c r="B78"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79"/>
-      <c r="B79"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80"/>
-      <c r="B80"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81"/>
-      <c r="B81"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82"/>
-      <c r="B82"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83"/>
-      <c r="B83"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84"/>
-      <c r="B84"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85"/>
-      <c r="B85"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86"/>
-      <c r="B86"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87"/>
-      <c r="B87"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88"/>
-      <c r="B88"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89"/>
-      <c r="B89"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90"/>
-      <c r="B90"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91"/>
-      <c r="B91"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92"/>
-      <c r="B92"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93"/>
-      <c r="B93"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94"/>
-      <c r="B94"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95"/>
-      <c r="B95"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96"/>
-      <c r="B96"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97"/>
-      <c r="B97"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98"/>
-      <c r="B98"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99"/>
-      <c r="B99"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100"/>
-      <c r="B100"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101"/>
-      <c r="B101"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102"/>
-      <c r="B102"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103"/>
-      <c r="B103"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104"/>
-      <c r="B104"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105"/>
-      <c r="B105"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106"/>
-      <c r="B106"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107"/>
-      <c r="B107"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108"/>
-      <c r="B108"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109"/>
-      <c r="B109"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110"/>
-      <c r="B110"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111"/>
-      <c r="B111"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112"/>
-      <c r="B112"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113"/>
-      <c r="B113"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114"/>
-      <c r="B114"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115"/>
-      <c r="B115"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116"/>
-      <c r="B116"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117"/>
-      <c r="B117"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118"/>
-      <c r="B118"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119"/>
-      <c r="B119"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120"/>
-      <c r="B120"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121"/>
-      <c r="B121"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122"/>
-      <c r="B122"/>
-    </row>
-  </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A23"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>